<commit_message>
FIX: R3/TO matrix missing a few entries.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="181">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -550,6 +550,18 @@
   </si>
   <si>
     <t>function/</t>
+  </si>
+  <si>
+    <t>base 16 bbinary to number</t>
+  </si>
+  <si>
+    <t>to char! FIRST binary</t>
+  </si>
+  <si>
+    <t>bytes to tuple</t>
+  </si>
+  <si>
+    <t>MAKE bitset! binary</t>
   </si>
 </sst>
 </file>
@@ -3864,7 +3876,7 @@
   <dimension ref="B3:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4295,10 +4307,16 @@
       <c r="B14" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+      <c r="C14" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>179</v>
+      </c>
       <c r="G14" s="27" t="s">
         <v>121</v>
       </c>
@@ -4306,8 +4324,10 @@
         <v>1</v>
       </c>
       <c r="I14" s="29"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="28" t="s">
+        <v>180</v>
+      </c>
       <c r="L14" s="27" t="s">
         <v>127</v>
       </c>

</xml_diff>

<commit_message>
FIX: few fixes to the R3 TO matrix.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -14,8 +14,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>dk</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2:
+TRUE =&gt; 1
+ FALSE =&gt; 0
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="180">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -379,10 +416,6 @@
     <t>FIRST string</t>
   </si>
   <si>
-    <t>TRUE =&gt; 1
- FALSE =&gt; 0</t>
-  </si>
-  <si>
     <t>NONE</t>
   </si>
   <si>
@@ -552,9 +585,6 @@
     <t>function/</t>
   </si>
   <si>
-    <t>base 16 bbinary to number</t>
-  </si>
-  <si>
     <t>to char! FIRST binary</t>
   </si>
   <si>
@@ -562,13 +592,16 @@
   </si>
   <si>
     <t>MAKE bitset! binary</t>
+  </si>
+  <si>
+    <t>base 16 binary to number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -589,6 +622,19 @@
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3872,11 +3918,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3958,7 +4004,7 @@
       </c>
       <c r="F4" s="29"/>
       <c r="G4" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" s="27" t="b">
         <v>1</v>
@@ -3966,23 +4012,23 @@
       <c r="I4" s="29"/>
       <c r="J4" s="29"/>
       <c r="K4" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L4" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="M4" s="27" t="s">
         <v>127</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>128</v>
       </c>
       <c r="N4" s="29"/>
       <c r="O4" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="P4" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q4" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R4" s="29"/>
       <c r="T4" s="26"/>
@@ -4001,7 +4047,7 @@
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
       <c r="G5" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H5" s="27" t="b">
         <v>1</v>
@@ -4010,18 +4056,18 @@
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
       <c r="L5" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M5" s="29"/>
       <c r="N5" s="29"/>
       <c r="O5" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q5" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R5" s="29"/>
       <c r="T5" s="29"/>
@@ -4040,7 +4086,7 @@
       <c r="E6" s="26"/>
       <c r="F6" s="29"/>
       <c r="G6" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" s="27" t="b">
         <v>1</v>
@@ -4048,25 +4094,25 @@
       <c r="I6" s="29"/>
       <c r="J6" s="29"/>
       <c r="K6" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M6" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q6" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R6" s="29"/>
     </row>
@@ -4079,7 +4125,7 @@
       <c r="E7" s="29"/>
       <c r="F7" s="26"/>
       <c r="G7" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H7" s="27" t="b">
         <v>1</v>
@@ -4088,20 +4134,20 @@
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
       <c r="L7" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M7" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N7" s="29"/>
       <c r="O7" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P7" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q7" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R7" s="29"/>
     </row>
@@ -4121,16 +4167,16 @@
       <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M8" s="29"/>
       <c r="N8" s="29"/>
       <c r="O8" s="29"/>
       <c r="P8" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q8" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R8" s="29"/>
     </row>
@@ -4138,34 +4184,32 @@
       <c r="B9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>120</v>
-      </c>
+      <c r="C9" s="29"/>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
       <c r="K9" s="29"/>
       <c r="L9" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M9" s="29"/>
       <c r="N9" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O9" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P9" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q9" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R9" s="29"/>
     </row>
@@ -4178,7 +4222,7 @@
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="27" t="b">
         <v>1</v>
@@ -4187,20 +4231,20 @@
       <c r="J10" s="29"/>
       <c r="K10" s="29"/>
       <c r="L10" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M10" s="29"/>
       <c r="N10" s="27" t="s">
         <v>113</v>
       </c>
       <c r="O10" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P10" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q10" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R10" s="29"/>
     </row>
@@ -4213,7 +4257,7 @@
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="27" t="b">
         <v>1</v>
@@ -4222,18 +4266,18 @@
       <c r="J11" s="26"/>
       <c r="K11" s="29"/>
       <c r="L11" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M11" s="29"/>
       <c r="N11" s="29"/>
       <c r="O11" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P11" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q11" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R11" s="29"/>
     </row>
@@ -4246,7 +4290,7 @@
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H12" s="27" t="b">
         <v>1</v>
@@ -4255,20 +4299,20 @@
       <c r="J12" s="29"/>
       <c r="K12" s="26"/>
       <c r="L12" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M12" s="27" t="s">
         <v>113</v>
       </c>
       <c r="N12" s="29"/>
       <c r="O12" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P12" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q12" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R12" s="29"/>
     </row>
@@ -4281,7 +4325,7 @@
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H13" s="27" t="b">
         <v>1</v>
@@ -4293,13 +4337,13 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
       <c r="O13" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P13" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q13" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R13" s="29"/>
     </row>
@@ -4308,17 +4352,17 @@
         <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H14" s="27" t="b">
         <v>1</v>
@@ -4326,21 +4370,21 @@
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
       <c r="K14" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L14" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M14" s="26"/>
       <c r="N14" s="29"/>
       <c r="O14" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P14" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q14" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R14" s="29"/>
     </row>
@@ -4353,7 +4397,7 @@
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H15" s="27" t="b">
         <v>1</v>
@@ -4362,18 +4406,18 @@
       <c r="J15" s="29"/>
       <c r="K15" s="29"/>
       <c r="L15" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M15" s="29"/>
       <c r="N15" s="26"/>
       <c r="O15" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P15" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q15" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R15" s="29"/>
     </row>
@@ -4394,7 +4438,7 @@
         <v>118</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H16" s="27" t="b">
         <v>1</v>
@@ -4402,13 +4446,13 @@
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L16" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M16" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N16" s="27" t="s">
         <v>113</v>
@@ -4418,7 +4462,7 @@
         <v>118</v>
       </c>
       <c r="Q16" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="R16" s="29"/>
     </row>
@@ -4433,31 +4477,31 @@
         <v>117</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H17" s="27" t="b">
         <v>1</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K17" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="L17" s="27" t="s">
-        <v>127</v>
-      </c>
       <c r="M17" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N17" s="29"/>
       <c r="O17" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P17" s="26"/>
       <c r="Q17" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R17" s="29"/>
     </row>
@@ -4470,7 +4514,7 @@
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="27" t="b">
         <v>1</v>
@@ -4479,15 +4523,15 @@
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
       <c r="O18" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P18" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q18" s="26"/>
       <c r="R18" s="29"/>
@@ -4501,7 +4545,7 @@
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
       <c r="G19" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H19" s="27" t="b">
         <v>1</v>
@@ -4510,23 +4554,24 @@
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
       <c r="O19" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P19" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q19" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R19" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT: completed "R3 TO matrix".
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -20,7 +20,32 @@
     <author>dk</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0">
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+truncates decimals if any
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="194">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -373,9 +398,6 @@
     <t>any-string!</t>
   </si>
   <si>
-    <t>number!</t>
-  </si>
-  <si>
     <t>any-list!</t>
   </si>
   <si>
@@ -391,13 +413,7 @@
     <t>convert to seconds</t>
   </si>
   <si>
-    <t>codepoint to number</t>
-  </si>
-  <si>
     <t>direct</t>
-  </si>
-  <si>
-    <t>number to codepoint</t>
   </si>
   <si>
     <t>No conversion required</t>
@@ -410,9 +426,6 @@
 to tuple</t>
   </si>
   <si>
-    <t>LOAD string</t>
-  </si>
-  <si>
     <t>FIRST string</t>
   </si>
   <si>
@@ -422,9 +435,6 @@
     <t>list of datatype names or values to typeset</t>
   </si>
   <si>
-    <t>MAKE bitset! number</t>
-  </si>
-  <si>
     <t>MAKE bitset! char</t>
   </si>
   <si>
@@ -435,9 +445,6 @@
   </si>
   <si>
     <t>UNSET</t>
-  </si>
-  <si>
-    <t>number to binary in base 16</t>
   </si>
   <si>
     <t>codepoint to binary in base 16</t>
@@ -459,9 +466,6 @@
 FALSE =&gt; 'FALSE</t>
   </si>
   <si>
-    <t>FORM number</t>
-  </si>
-  <si>
     <t>FORM time</t>
   </si>
   <si>
@@ -501,9 +505,6 @@
     <t>FORM function</t>
   </si>
   <si>
-    <t>[number]</t>
-  </si>
-  <si>
     <t>[time]</t>
   </si>
   <si>
@@ -549,9 +550,6 @@
     <t>list values to path</t>
   </si>
   <si>
-    <t>number/</t>
-  </si>
-  <si>
     <t>time/</t>
   </si>
   <si>
@@ -594,14 +592,83 @@
     <t>MAKE bitset! binary</t>
   </si>
   <si>
-    <t>base 16 binary to number</t>
+    <t>truncate</t>
+  </si>
+  <si>
+    <t>integer to seconds</t>
+  </si>
+  <si>
+    <t>integer  to codepoint</t>
+  </si>
+  <si>
+    <t>MAKE bitset! Integer</t>
+  </si>
+  <si>
+    <t>FORM integer</t>
+  </si>
+  <si>
+    <t>[integer]</t>
+  </si>
+  <si>
+    <t>integer/</t>
+  </si>
+  <si>
+    <t>decimal to seconds with decimals</t>
+  </si>
+  <si>
+    <t>truncate decimal to codepoint</t>
+  </si>
+  <si>
+    <t>decimal in base 16 binary</t>
+  </si>
+  <si>
+    <t>integer in base 16 binary</t>
+  </si>
+  <si>
+    <t>FORM decimal</t>
+  </si>
+  <si>
+    <t>[decimal]</t>
+  </si>
+  <si>
+    <t>decimal/</t>
+  </si>
+  <si>
+    <t>convert to seconds with decimals</t>
+  </si>
+  <si>
+    <t>codepoint to decimal number</t>
+  </si>
+  <si>
+    <t>codepoint to integer</t>
+  </si>
+  <si>
+    <t>base 16 binary as integer</t>
+  </si>
+  <si>
+    <t>base 16 binary as decimal</t>
+  </si>
+  <si>
+    <t>LOAD string as integer</t>
+  </si>
+  <si>
+    <t>LOAD string as decimal</t>
+  </si>
+  <si>
+    <t>LOAD string as time</t>
+  </si>
+  <si>
+    <t>LOAD string as tuple</t>
+  </si>
+  <si>
+    <t>LOAD string as list</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -635,6 +702,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -864,18 +944,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -905,6 +973,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2110,66 +2190,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="18"/>
-      <c r="BF1" s="18"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
+      <c r="AQ1" s="28"/>
+      <c r="AR1" s="28"/>
+      <c r="AS1" s="28"/>
+      <c r="AT1" s="28"/>
+      <c r="AU1" s="28"/>
+      <c r="AV1" s="28"/>
+      <c r="AW1" s="28"/>
+      <c r="AX1" s="28"/>
+      <c r="AY1" s="28"/>
+      <c r="AZ1" s="28"/>
+      <c r="BA1" s="28"/>
+      <c r="BB1" s="28"/>
+      <c r="BC1" s="28"/>
+      <c r="BD1" s="28"/>
+      <c r="BE1" s="28"/>
+      <c r="BF1" s="28"/>
     </row>
     <row r="2" spans="1:58" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2346,7 +2426,7 @@
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2522,7 +2602,7 @@
       </c>
     </row>
     <row r="4" spans="1:58" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
         <v>61</v>
@@ -2622,7 +2702,7 @@
       <c r="BF4" s="9"/>
     </row>
     <row r="5" spans="1:58" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2798,7 +2878,7 @@
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="7"/>
       <c r="C6" s="12"/>
       <c r="D6" s="9"/>
@@ -3919,655 +3999,724 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:U19"/>
+  <dimension ref="B3:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="13" width="11.85546875" style="22" customWidth="1"/>
-    <col min="14" max="14" width="14" style="22" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="22" customWidth="1"/>
-    <col min="16" max="17" width="11.85546875" style="22" customWidth="1"/>
-    <col min="18" max="18" width="13.28515625" style="22" customWidth="1"/>
+    <col min="3" max="14" width="11.85546875" style="18" customWidth="1"/>
+    <col min="15" max="15" width="14" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+    <row r="3" spans="2:22" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="R4" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="S4" s="25"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="P5" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="R5" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="S5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="D6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="S6" s="25"/>
+    </row>
+    <row r="7" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="R7" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="S7" s="25"/>
+    </row>
+    <row r="8" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O8" s="25"/>
+      <c r="P8" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="R8" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="S8" s="25"/>
+    </row>
+    <row r="9" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="R9" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="S9" s="25"/>
+    </row>
+    <row r="10" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" s="25"/>
+      <c r="O10" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q10" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="S10" s="25"/>
+    </row>
+    <row r="11" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="25"/>
+      <c r="O11" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q11" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="R11" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="S11" s="25"/>
+    </row>
+    <row r="12" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q12" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="R12" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="S12" s="25"/>
+    </row>
+    <row r="13" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q13" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="R13" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="S13" s="25"/>
+    </row>
+    <row r="14" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q14" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="R14" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="S14" s="25"/>
+    </row>
+    <row r="15" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="R15" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="S15" s="25"/>
+    </row>
+    <row r="16" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N16" s="25"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q16" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="R17" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="S17" s="25"/>
+    </row>
+    <row r="18" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="P3" s="24" t="s">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M18" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="O18" s="25"/>
+      <c r="P18" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="S18" s="25"/>
+    </row>
+    <row r="19" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="Q3" s="24" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q19" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="R19" s="22"/>
+      <c r="S19" s="25"/>
+    </row>
+    <row r="20" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="R3" s="24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="27" t="b">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="23" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="N4" s="29"/>
-      <c r="O4" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="P4" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="R4" s="29"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="P5" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q5" s="27" t="s">
-        <v>165</v>
-      </c>
-      <c r="R5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H6" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="L6" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M6" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="O6" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="P6" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q6" s="27" t="s">
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q20" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="R20" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="R6" s="29"/>
-    </row>
-    <row r="7" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H7" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M7" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="N7" s="29"/>
-      <c r="O7" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="P7" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q7" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="R7" s="29"/>
-    </row>
-    <row r="8" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q8" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="R8" s="29"/>
-    </row>
-    <row r="9" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="O9" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="P9" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q9" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="R9" s="29"/>
-    </row>
-    <row r="10" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H10" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="O10" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="P10" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q10" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="R10" s="29"/>
-    </row>
-    <row r="11" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H11" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q11" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="R11" s="29"/>
-    </row>
-    <row r="12" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H12" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M12" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="P12" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q12" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="R12" s="29"/>
-    </row>
-    <row r="13" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H13" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="P13" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q13" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="R13" s="29"/>
-    </row>
-    <row r="14" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="L14" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M14" s="26"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="P14" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q14" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="R14" s="29"/>
-    </row>
-    <row r="15" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="P15" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q15" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="R15" s="29"/>
-    </row>
-    <row r="16" spans="2:21" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="L16" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M16" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="N16" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="O16" s="26"/>
-      <c r="P16" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q16" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="R16" s="29"/>
-    </row>
-    <row r="17" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H17" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="K17" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="L17" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M17" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="N17" s="29"/>
-      <c r="O17" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="27" t="s">
-        <v>163</v>
-      </c>
-      <c r="R17" s="29"/>
-    </row>
-    <row r="18" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H18" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29"/>
-      <c r="O18" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="P18" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="29"/>
-    </row>
-    <row r="19" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="H19" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="P19" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q19" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="R19" s="29"/>
+      <c r="S20" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FEAT: adds MAKE matrix for R3.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - Red Datatype Comparis" sheetId="1" r:id="rId1"/>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId2"/>
+    <sheet name="R3 MAKE matrix" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -76,8 +77,144 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>dk</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+truncates decimals if any
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Forbidden if empty cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+R2: empty block
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R2: empty path
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2:
+TRUE =&gt; 1
+ FALSE =&gt; 0
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="207">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -662,6 +799,47 @@
   </si>
   <si>
     <t>LOAD string as list</t>
+  </si>
+  <si>
+    <t>&lt;&gt; 0 =&gt; TRUE
+= 0 =&gt; FALSE</t>
+  </si>
+  <si>
+    <t>Difference with TO</t>
+  </si>
+  <si>
+    <t>&lt;&gt; 0.0 =&gt; TRUE
+= 0.0 =&gt; FALSE</t>
+  </si>
+  <si>
+    <t>New binary with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New binary with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with (binary to integer) slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with (binary to integer) slots preallocated</t>
   </si>
 </sst>
 </file>
@@ -717,7 +895,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,6 +929,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -889,7 +1073,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -984,6 +1168,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4001,15 +4191,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="14" width="11.85546875" style="18" customWidth="1"/>
+    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="18" customWidth="1"/>
     <col min="15" max="15" width="14" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="18" width="11.85546875" style="18" customWidth="1"/>
@@ -4723,4 +4914,693 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:V20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
+    <col min="14" max="15" width="14" style="18" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="18" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" style="18" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" style="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:22" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q3" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="R3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="S3" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="R4" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="S4" s="25"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="P5" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="R5" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="S5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="25"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="25"/>
+    </row>
+    <row r="8" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O8" s="25"/>
+      <c r="P8" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="25"/>
+    </row>
+    <row r="9" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="25"/>
+    </row>
+    <row r="10" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" s="25"/>
+      <c r="O10" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="P10" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="25"/>
+    </row>
+    <row r="11" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N11" s="25"/>
+      <c r="O11" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="25"/>
+    </row>
+    <row r="12" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I12" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="25"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="25"/>
+    </row>
+    <row r="13" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N13" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="O13" s="25"/>
+      <c r="P13" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="25"/>
+    </row>
+    <row r="14" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="25"/>
+    </row>
+    <row r="15" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q15" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="R15" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="S15" s="25"/>
+    </row>
+    <row r="16" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N16" s="25"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="M17" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N17" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="R17" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="S17" s="25"/>
+    </row>
+    <row r="18" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M18" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="O18" s="25"/>
+      <c r="P18" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="S18" s="25"/>
+    </row>
+    <row r="19" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q19" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="R19" s="22"/>
+      <c r="S19" s="25"/>
+    </row>
+    <row r="20" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: minor fixes to R3 MAKE matrix.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -21,6 +21,33 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="I4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2:
+&lt;&gt; 0 =&gt; TRUE
+0 =&gt; FALSE
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C6" authorId="0">
       <text>
         <r>
@@ -182,39 +209,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>dk:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-In R2:
-TRUE =&gt; 1
- FALSE =&gt; 0
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="208">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -801,45 +801,49 @@
     <t>LOAD string as list</t>
   </si>
   <si>
+    <t>Difference with TO</t>
+  </si>
+  <si>
+    <t>New binary with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New binary with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with truncated decimal slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with (binary to integer) slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with (binary to integer) slots preallocated</t>
+  </si>
+  <si>
+    <t>TRUE =&gt; 1
+ FALSE =&gt; 0</t>
+  </si>
+  <si>
     <t>&lt;&gt; 0 =&gt; TRUE
-= 0 =&gt; FALSE</t>
-  </si>
-  <si>
-    <t>Difference with TO</t>
+0 =&gt; FALSE</t>
   </si>
   <si>
     <t>&lt;&gt; 0.0 =&gt; TRUE
-= 0.0 =&gt; FALSE</t>
-  </si>
-  <si>
-    <t>New binary with integer slots preallocated</t>
-  </si>
-  <si>
-    <t>New binary with truncated decimal slots preallocated</t>
-  </si>
-  <si>
-    <t>New string with integer slots preallocated</t>
-  </si>
-  <si>
-    <t>New list with integer slots preallocated</t>
-  </si>
-  <si>
-    <t>New path with integer slots preallocated</t>
-  </si>
-  <si>
-    <t>New string with truncated decimal slots preallocated</t>
-  </si>
-  <si>
-    <t>New list with truncated decimal slots preallocated</t>
-  </si>
-  <si>
-    <t>New path with truncated decimal slots preallocated</t>
-  </si>
-  <si>
-    <t>New list with (binary to integer) slots preallocated</t>
-  </si>
-  <si>
-    <t>New path with (binary to integer) slots preallocated</t>
+0.0 =&gt; FALSE</t>
   </si>
 </sst>
 </file>
@@ -4192,7 +4196,7 @@
   <dimension ref="B3:V20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4921,7 +4925,7 @@
   <dimension ref="B3:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5011,7 +5015,7 @@
         <v>116</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
@@ -5022,17 +5026,17 @@
         <v>121</v>
       </c>
       <c r="N4" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="R4" s="32" t="s">
         <v>199</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="R4" s="32" t="s">
-        <v>201</v>
       </c>
       <c r="S4" s="25"/>
       <c r="U4" s="22"/>
@@ -5059,7 +5063,7 @@
         <v>116</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -5068,17 +5072,17 @@
         <v>121</v>
       </c>
       <c r="N5" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="R5" s="32" t="s">
         <v>202</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="R5" s="32" t="s">
-        <v>204</v>
       </c>
       <c r="S5" s="25"/>
       <c r="U5" s="25"/>
@@ -5121,7 +5125,7 @@
       <c r="S6" s="25"/>
       <c r="U6" s="33"/>
       <c r="V6" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5226,7 +5230,9 @@
       <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="32" t="s">
+        <v>205</v>
+      </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
@@ -5411,10 +5417,10 @@
         <v>136</v>
       </c>
       <c r="Q15" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R15" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="S15" s="25"/>
     </row>

</xml_diff>

<commit_message>
FIX: change decimal! to any-float! in the Red matrices.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="242">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -1296,6 +1296,57 @@
   </si>
   <si>
     <t>object/</t>
+  </si>
+  <si>
+    <t>any-float!</t>
+  </si>
+  <si>
+    <t>any-float to seconds with decimals</t>
+  </si>
+  <si>
+    <t>truncate any-float to codepoint</t>
+  </si>
+  <si>
+    <t>any-float in base 16 binary</t>
+  </si>
+  <si>
+    <t>FORM any-float</t>
+  </si>
+  <si>
+    <t>[any-float]</t>
+  </si>
+  <si>
+    <t>any-float/</t>
+  </si>
+  <si>
+    <t>codepoint to any-float number</t>
+  </si>
+  <si>
+    <t>base 16 binary as any-float</t>
+  </si>
+  <si>
+    <t>LOAD string as any-float</t>
+  </si>
+  <si>
+    <t>New binary with truncated any-float slots preallocated</t>
+  </si>
+  <si>
+    <t>New string with truncated any-float slots preallocated</t>
+  </si>
+  <si>
+    <t>New list with truncated any-float slots preallocated</t>
+  </si>
+  <si>
+    <t>New path with truncated any-float slots preallocated</t>
+  </si>
+  <si>
+    <t>truncated any-float to codepoint</t>
+  </si>
+  <si>
+    <t>New map with truncated any-float slots preallocated</t>
+  </si>
+  <si>
+    <t>New vector with truncated any-float slots preallocated</t>
   </si>
 </sst>
 </file>
@@ -4624,8 +4675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4648,7 +4699,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -4758,17 +4809,17 @@
     </row>
     <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>170</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -4784,17 +4835,17 @@
         <v>121</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="23" t="s">
-        <v>181</v>
+        <v>229</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>183</v>
+        <v>231</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
@@ -4854,7 +4905,7 @@
         <v>186</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -5162,7 +5213,7 @@
         <v>187</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -5248,7 +5299,7 @@
         <v>189</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>191</v>
@@ -5539,7 +5590,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5549,7 +5600,7 @@
     <col min="3" max="13" width="11.85546875" style="18" customWidth="1"/>
     <col min="14" max="15" width="14" style="18" customWidth="1"/>
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="18" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
     <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
   </cols>
@@ -5562,7 +5613,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -5676,17 +5727,17 @@
     </row>
     <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>170</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>178</v>
+        <v>239</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -5702,25 +5753,25 @@
         <v>121</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="28" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
       <c r="Q5" s="28" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
       <c r="R5" s="28" t="s">
-        <v>202</v>
+        <v>238</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="28" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="V5" s="28" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="X5" s="25"/>
       <c r="Y5" s="27" t="s">
@@ -5776,7 +5827,7 @@
         <v>186</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -6052,7 +6103,7 @@
         <v>187</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -6132,7 +6183,7 @@
         <v>189</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>191</v>

</xml_diff>

<commit_message>
FIX: minor improvements for bitset! in conversion matrices.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -46,6 +46,31 @@
 In R2:
 &lt;&gt; 0 =&gt; TRUE
 0 =&gt; FALSE
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rounded up to multiple of 8
 </t>
         </r>
       </text>
@@ -162,6 +187,31 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rounded up to multiple of 8
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C6" authorId="0">
       <text>
         <r>
@@ -348,6 +398,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rounded up to multiple of 8
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C6" authorId="0">
       <text>
         <r>
@@ -460,6 +535,31 @@
     <author>dk</author>
   </authors>
   <commentList>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rounded up to multiple of 8
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C6" authorId="0">
       <text>
         <r>
@@ -1139,9 +1239,6 @@
     <t>integer  to codepoint</t>
   </si>
   <si>
-    <t>MAKE bitset! Integer</t>
-  </si>
-  <si>
     <t>FORM integer</t>
   </si>
   <si>
@@ -1304,9 +1401,6 @@
     <t>any-float to seconds with decimals</t>
   </si>
   <si>
-    <t>truncate any-float to codepoint</t>
-  </si>
-  <si>
     <t>any-float in base 16 binary</t>
   </si>
   <si>
@@ -1347,6 +1441,12 @@
   </si>
   <si>
     <t>New vector with truncated any-float slots preallocated</t>
+  </si>
+  <si>
+    <t>New bitset with integer slots preallocated</t>
+  </si>
+  <si>
+    <t>MAKE tuple! list</t>
   </si>
 </sst>
 </file>
@@ -2874,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21:Q23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2979,23 +3079,23 @@
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q4" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>175</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>176</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
@@ -3015,10 +3115,10 @@
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>177</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>178</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -3034,17 +3134,17 @@
         <v>121</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q5" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="R5" s="23" t="s">
         <v>182</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>183</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
@@ -3063,7 +3163,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -3101,10 +3201,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -3346,7 +3446,7 @@
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
       <c r="L13" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M13" s="23" t="s">
         <v>121</v>
@@ -3409,10 +3509,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>187</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>188</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -3436,7 +3536,7 @@
         <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
@@ -3495,19 +3595,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="E17" s="23" t="s">
         <v>190</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>191</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -3530,10 +3630,10 @@
         <v>111</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R17" s="23" t="s">
         <v>154</v>
@@ -3552,7 +3652,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
-        <v>114</v>
+        <v>241</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>116</v>
@@ -3578,7 +3678,7 @@
         <v>138</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R18" s="23" t="s">
         <v>155</v>
@@ -3586,7 +3686,7 @@
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V18" s="25"/>
     </row>
@@ -3620,7 +3720,7 @@
         <v>152</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
@@ -3688,13 +3788,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q21" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="R21" s="23" t="s">
         <v>208</v>
-      </c>
-      <c r="Q21" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>209</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
@@ -3728,15 +3828,15 @@
         <v>140</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
       <c r="U22" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V22" s="25"/>
     </row>
@@ -3767,10 +3867,10 @@
         <v>140</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -3788,8 +3888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21:Q23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3888,36 +3988,36 @@
         <v>116</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q4" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="R4" s="28" t="s">
         <v>198</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>199</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" s="28" t="s">
         <v>212</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>213</v>
       </c>
       <c r="X4" s="22"/>
       <c r="Y4" s="26" t="s">
@@ -3933,17 +4033,17 @@
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>177</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>178</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -3952,25 +4052,25 @@
         <v>121</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q5" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="R5" s="28" t="s">
         <v>201</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>202</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="V5" s="28" t="s">
         <v>214</v>
-      </c>
-      <c r="V5" s="28" t="s">
-        <v>215</v>
       </c>
       <c r="X5" s="25"/>
       <c r="Y5" s="27" t="s">
@@ -3985,7 +4085,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -4015,7 +4115,7 @@
       <c r="V6" s="25"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4023,10 +4123,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -4130,7 +4230,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -4299,10 +4399,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>187</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>188</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -4331,10 +4431,10 @@
         <v>136</v>
       </c>
       <c r="Q15" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="R15" s="28" t="s">
         <v>203</v>
-      </c>
-      <c r="R15" s="28" t="s">
-        <v>204</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -4379,19 +4479,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="E17" s="23" t="s">
         <v>190</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>191</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -4415,7 +4515,7 @@
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R17" s="23" t="s">
         <v>154</v>
@@ -4466,10 +4566,10 @@
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="V18" s="28" t="s">
         <v>216</v>
-      </c>
-      <c r="V18" s="28" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4564,13 +4664,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q21" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="R21" s="23" t="s">
         <v>208</v>
-      </c>
-      <c r="Q21" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>209</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
@@ -4607,17 +4707,17 @@
         <v>140</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U22" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V22" s="25"/>
       <c r="W22" s="34"/>
@@ -4651,10 +4751,10 @@
         <v>140</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -4675,8 +4775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4699,7 +4799,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -4780,23 +4880,23 @@
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q4" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>175</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>176</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
@@ -4809,17 +4909,17 @@
     </row>
     <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>170</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -4835,17 +4935,17 @@
         <v>121</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="R5" s="23" t="s">
         <v>229</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>231</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
@@ -4864,7 +4964,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -4902,10 +5002,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -5147,7 +5247,7 @@
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
       <c r="L13" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M13" s="23" t="s">
         <v>121</v>
@@ -5210,10 +5310,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -5237,7 +5337,7 @@
         <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
@@ -5296,19 +5396,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -5331,10 +5431,10 @@
         <v>111</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R17" s="23" t="s">
         <v>154</v>
@@ -5353,7 +5453,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
-        <v>114</v>
+        <v>241</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>116</v>
@@ -5379,7 +5479,7 @@
         <v>138</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R18" s="23" t="s">
         <v>155</v>
@@ -5387,7 +5487,7 @@
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="V18" s="25"/>
     </row>
@@ -5421,7 +5521,7 @@
         <v>152</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
@@ -5489,13 +5589,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
@@ -5529,15 +5629,15 @@
         <v>140</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
       <c r="U22" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V22" s="25"/>
     </row>
@@ -5568,10 +5668,10 @@
         <v>140</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -5589,8 +5689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5602,7 +5702,9 @@
     <col min="16" max="16" width="13.7109375" style="18" customWidth="1"/>
     <col min="17" max="17" width="13.85546875" style="18" customWidth="1"/>
     <col min="18" max="18" width="13.7109375" style="18" customWidth="1"/>
-    <col min="19" max="22" width="13.28515625" style="18" customWidth="1"/>
+    <col min="19" max="20" width="13.28515625" style="18" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="18" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:25" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5613,7 +5715,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -5689,36 +5791,36 @@
         <v>116</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q4" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="R4" s="28" t="s">
         <v>198</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>199</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="V4" s="28" t="s">
         <v>212</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>213</v>
       </c>
       <c r="X4" s="22"/>
       <c r="Y4" s="26" t="s">
@@ -5727,24 +5829,24 @@
     </row>
     <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>170</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -5753,25 +5855,25 @@
         <v>121</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="R5" s="28" t="s">
         <v>236</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>238</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="V5" s="28" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="X5" s="25"/>
       <c r="Y5" s="27" t="s">
@@ -5786,7 +5888,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -5816,7 +5918,7 @@
       <c r="V6" s="25"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5824,10 +5926,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -5931,7 +6033,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -6100,10 +6202,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
@@ -6132,10 +6234,10 @@
         <v>136</v>
       </c>
       <c r="Q15" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="R15" s="28" t="s">
         <v>203</v>
-      </c>
-      <c r="R15" s="28" t="s">
-        <v>204</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -6180,19 +6282,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -6216,7 +6318,7 @@
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R17" s="23" t="s">
         <v>154</v>
@@ -6267,10 +6369,10 @@
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="V18" s="28" t="s">
         <v>216</v>
-      </c>
-      <c r="V18" s="28" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -6365,10 +6467,10 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R21" s="28"/>
       <c r="S21" s="25"/>
@@ -6406,15 +6508,15 @@
         <v>140</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R22" s="28"/>
       <c r="S22" s="25"/>
       <c r="T22" s="28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="U22" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V22" s="25"/>
       <c r="W22" s="34"/>
@@ -6448,10 +6550,10 @@
         <v>140</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>

</xml_diff>

<commit_message>
FIX: minor cosmetics changes.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -1771,6 +1771,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1782,9 +1785,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4676,9 +4676,9 @@
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="30"/>
     </row>
     <row r="22" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
@@ -4720,9 +4720,9 @@
         <v>209</v>
       </c>
       <c r="V22" s="25"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
     </row>
     <row r="23" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
@@ -4760,9 +4760,9 @@
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4776,7 +4776,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6477,9 +6477,9 @@
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="25"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="30"/>
     </row>
     <row r="22" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
@@ -6519,9 +6519,9 @@
         <v>209</v>
       </c>
       <c r="V22" s="25"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="30"/>
     </row>
     <row r="23" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
@@ -6559,9 +6559,9 @@
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="34"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6590,66 +6590,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="30"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="30"/>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
+      <c r="BE1" s="31"/>
+      <c r="BF1" s="31"/>
     </row>
     <row r="2" spans="1:58" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -6826,7 +6826,7 @@
       </c>
     </row>
     <row r="3" spans="1:58" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -7002,7 +7002,7 @@
       </c>
     </row>
     <row r="4" spans="1:58" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
         <v>61</v>
@@ -7102,7 +7102,7 @@
       <c r="BF4" s="9"/>
     </row>
     <row r="5" spans="1:58" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -7278,7 +7278,7 @@
       </c>
     </row>
     <row r="6" spans="1:58" ht="68.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="7"/>
       <c r="C6" s="12"/>
       <c r="D6" s="9"/>

</xml_diff>

<commit_message>
FEAT: adds comment for "to word! logic" conversions.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -123,6 +123,31 @@
 In R2:
 TRUE =&gt; 1
  FALSE =&gt; 0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: forbidden
 </t>
         </r>
       </text>
@@ -308,6 +333,30 @@
           <t xml:space="preserve">
 R2: empty path
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In R2: forbidden</t>
         </r>
       </text>
     </comment>
@@ -2975,7 +3024,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3888,8 +3937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4775,8 +4824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
FIX: forbids bitset to bitset conversions in R3 TO/MAKE matrices.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -764,7 +764,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="242">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -3024,7 +3024,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3494,9 +3494,7 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="22" t="s">
-        <v>209</v>
-      </c>
+      <c r="L13" s="25"/>
       <c r="M13" s="23" t="s">
         <v>121</v>
       </c>
@@ -3937,8 +3935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4394,7 +4392,7 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="22"/>
+      <c r="L13" s="25"/>
       <c r="M13" s="23" t="s">
         <v>121</v>
       </c>
@@ -4824,8 +4822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5739,7 +5737,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6197,7 +6195,9 @@
       </c>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="22"/>
+      <c r="L13" s="22" t="s">
+        <v>209</v>
+      </c>
       <c r="M13" s="23" t="s">
         <v>121</v>
       </c>
@@ -6277,7 +6277,9 @@
       <c r="M15" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="N15" s="22"/>
+      <c r="N15" s="22" t="s">
+        <v>209</v>
+      </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
         <v>136</v>
@@ -6365,7 +6367,9 @@
       <c r="O17" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="P17" s="22"/>
+      <c r="P17" s="22" t="s">
+        <v>209</v>
+      </c>
       <c r="Q17" s="23" t="s">
         <v>192</v>
       </c>
@@ -6411,7 +6415,9 @@
       <c r="P18" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="Q18" s="22"/>
+      <c r="Q18" s="22" t="s">
+        <v>209</v>
+      </c>
       <c r="R18" s="23" t="s">
         <v>155</v>
       </c>
@@ -6453,7 +6459,9 @@
       <c r="Q19" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="R19" s="22"/>
+      <c r="R19" s="22" t="s">
+        <v>209</v>
+      </c>
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>

</xml_diff>

<commit_message>
FIX: improves any-string! to any-word! conversion description in matrices.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -764,7 +764,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="243">
   <si>
     <t>Red Datatype Comparison Matrix</t>
   </si>
@@ -1496,6 +1496,9 @@
   </si>
   <si>
     <t>MAKE tuple! list</t>
+  </si>
+  <si>
+    <t>LOAD string as any-word</t>
   </si>
 </sst>
 </file>
@@ -3024,7 +3027,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3674,7 +3677,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>209</v>
@@ -3936,7 +3939,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4558,7 +4561,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="23" t="s">
@@ -4822,8 +4825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5475,7 +5478,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>209</v>
@@ -5736,8 +5739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6365,7 +6368,7 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
FIX: improves binary! to any-string! description in conversion matrices.
</commit_message>
<xml_diff>
--- a/docs/to-datatype-matrix.xlsx
+++ b/docs/to-datatype-matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
     <sheet name="R3 TO matrix" sheetId="2" r:id="rId1"/>
@@ -1177,9 +1177,6 @@
     <t>FORM unset (empty string)</t>
   </si>
   <si>
-    <t>FORM binary (decode UTF-8)</t>
-  </si>
-  <si>
     <t>FORM word</t>
   </si>
   <si>
@@ -1499,6 +1496,9 @@
   </si>
   <si>
     <t>LOAD string as any-word</t>
+  </si>
+  <si>
+    <t>New string from binary (decode UTF-8)</t>
   </si>
 </sst>
 </file>
@@ -3026,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3116,10 +3116,10 @@
         <v>111</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>172</v>
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="23" t="s">
@@ -3131,23 +3131,23 @@
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q4" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>175</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
@@ -3163,14 +3163,14 @@
         <v>14</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>176</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>177</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -3186,17 +3186,17 @@
         <v>121</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q5" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="R5" s="23" t="s">
         <v>181</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>182</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
@@ -3215,7 +3215,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -3238,10 +3238,10 @@
         <v>128</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
@@ -3253,10 +3253,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -3285,10 +3285,10 @@
         <v>129</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S7" s="25"/>
       <c r="T7" s="25"/>
@@ -3324,10 +3324,10 @@
         <v>130</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
@@ -3357,10 +3357,10 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S9" s="25"/>
       <c r="T9" s="25"/>
@@ -3394,10 +3394,10 @@
         <v>131</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R10" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
@@ -3433,10 +3433,10 @@
         <v>132</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R11" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
@@ -3470,10 +3470,10 @@
         <v>134</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
@@ -3509,10 +3509,10 @@
         <v>133</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
@@ -3544,10 +3544,10 @@
         <v>135</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
@@ -3559,17 +3559,17 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>186</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>187</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>168</v>
       </c>
       <c r="H15" s="23" t="s">
         <v>116</v>
@@ -3580,23 +3580,23 @@
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M15" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>136</v>
+        <v>242</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R15" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -3627,13 +3627,13 @@
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S16" s="25"/>
       <c r="T16" s="25"/>
@@ -3645,19 +3645,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="E17" s="23" t="s">
         <v>189</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>190</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -3677,16 +3677,16 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
@@ -3702,7 +3702,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>116</v>
@@ -3725,18 +3725,18 @@
       </c>
       <c r="O18" s="25"/>
       <c r="P18" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V18" s="25"/>
     </row>
@@ -3764,13 +3764,13 @@
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
@@ -3801,13 +3801,13 @@
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R20" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S20" s="25"/>
       <c r="T20" s="25"/>
@@ -3838,13 +3838,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q21" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="R21" s="23" t="s">
         <v>207</v>
-      </c>
-      <c r="Q21" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>208</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
@@ -3875,18 +3875,18 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
       <c r="U22" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V22" s="25"/>
     </row>
@@ -3914,13 +3914,13 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -3939,7 +3939,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4028,46 +4028,46 @@
         <v>111</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>172</v>
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q4" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="R4" s="28" t="s">
         <v>197</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>198</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="V4" s="28" t="s">
         <v>211</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>212</v>
       </c>
       <c r="X4" s="22"/>
       <c r="Y4" s="26" t="s">
@@ -4079,21 +4079,21 @@
         <v>14</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>176</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>177</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -4102,25 +4102,25 @@
         <v>121</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q5" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="R5" s="28" t="s">
         <v>200</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>201</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="V5" s="28" t="s">
         <v>213</v>
-      </c>
-      <c r="V5" s="28" t="s">
-        <v>214</v>
       </c>
       <c r="X5" s="25"/>
       <c r="Y5" s="27" t="s">
@@ -4135,7 +4135,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -4165,7 +4165,7 @@
       <c r="V6" s="25"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4173,10 +4173,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -4280,7 +4280,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -4449,17 +4449,17 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>186</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>187</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>168</v>
       </c>
       <c r="H15" s="23" t="s">
         <v>116</v>
@@ -4470,7 +4470,7 @@
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M15" s="23" t="s">
         <v>121</v>
@@ -4478,13 +4478,13 @@
       <c r="N15" s="22"/>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>136</v>
+        <v>242</v>
       </c>
       <c r="Q15" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="R15" s="28" t="s">
         <v>202</v>
-      </c>
-      <c r="R15" s="28" t="s">
-        <v>203</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -4515,7 +4515,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q16" s="28"/>
       <c r="R16" s="28"/>
@@ -4529,19 +4529,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="E17" s="23" t="s">
         <v>189</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>190</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -4561,14 +4561,14 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P17" s="22"/>
       <c r="Q17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
@@ -4607,19 +4607,19 @@
       </c>
       <c r="O18" s="25"/>
       <c r="P18" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" s="22"/>
       <c r="R18" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="V18" s="28" t="s">
         <v>215</v>
-      </c>
-      <c r="V18" s="28" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4646,10 +4646,10 @@
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R19" s="22"/>
       <c r="S19" s="25"/>
@@ -4681,7 +4681,7 @@
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q20" s="28"/>
       <c r="R20" s="28"/>
@@ -4714,13 +4714,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q21" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="R21" s="23" t="s">
         <v>207</v>
-      </c>
-      <c r="Q21" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="R21" s="23" t="s">
-        <v>208</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
@@ -4754,20 +4754,20 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U22" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V22" s="25"/>
       <c r="W22" s="30"/>
@@ -4798,13 +4798,13 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -4826,7 +4826,7 @@
   <dimension ref="B3:Y23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4849,7 +4849,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -4915,10 +4915,10 @@
         <v>111</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>172</v>
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="23" t="s">
@@ -4930,23 +4930,23 @@
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q4" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>175</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
@@ -4959,17 +4959,17 @@
     </row>
     <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
@@ -4985,17 +4985,17 @@
         <v>121</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q5" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="Q5" s="23" t="s">
+      <c r="R5" s="23" t="s">
         <v>228</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>229</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
@@ -5014,7 +5014,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -5037,10 +5037,10 @@
         <v>128</v>
       </c>
       <c r="Q6" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S6" s="25"/>
       <c r="T6" s="25"/>
@@ -5052,10 +5052,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -5084,10 +5084,10 @@
         <v>129</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S7" s="25"/>
       <c r="T7" s="25"/>
@@ -5123,10 +5123,10 @@
         <v>130</v>
       </c>
       <c r="Q8" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R8" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S8" s="25"/>
       <c r="T8" s="25"/>
@@ -5156,10 +5156,10 @@
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
       <c r="Q9" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S9" s="25"/>
       <c r="T9" s="25"/>
@@ -5193,10 +5193,10 @@
         <v>131</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R10" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S10" s="25"/>
       <c r="T10" s="25"/>
@@ -5232,10 +5232,10 @@
         <v>132</v>
       </c>
       <c r="Q11" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R11" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S11" s="25"/>
       <c r="T11" s="25"/>
@@ -5269,10 +5269,10 @@
         <v>134</v>
       </c>
       <c r="Q12" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R12" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
@@ -5297,7 +5297,7 @@
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
       <c r="L13" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M13" s="23" t="s">
         <v>121</v>
@@ -5310,10 +5310,10 @@
         <v>133</v>
       </c>
       <c r="Q13" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R13" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
@@ -5345,10 +5345,10 @@
         <v>135</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S14" s="25"/>
       <c r="T14" s="25"/>
@@ -5360,17 +5360,17 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>168</v>
       </c>
       <c r="H15" s="23" t="s">
         <v>116</v>
@@ -5381,23 +5381,23 @@
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M15" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>136</v>
+        <v>242</v>
       </c>
       <c r="Q15" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R15" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -5428,13 +5428,13 @@
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q16" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R16" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S16" s="25"/>
       <c r="T16" s="25"/>
@@ -5446,19 +5446,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -5478,16 +5478,16 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
@@ -5503,7 +5503,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="25"/>
       <c r="G18" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>116</v>
@@ -5526,18 +5526,18 @@
       </c>
       <c r="O18" s="25"/>
       <c r="P18" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V18" s="25"/>
     </row>
@@ -5565,13 +5565,13 @@
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
@@ -5602,13 +5602,13 @@
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q20" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R20" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="S20" s="25"/>
       <c r="T20" s="25"/>
@@ -5639,13 +5639,13 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R21" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S21" s="25"/>
       <c r="T21" s="25"/>
@@ -5676,18 +5676,18 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R22" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
       <c r="U22" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V22" s="25"/>
     </row>
@@ -5715,13 +5715,13 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
@@ -5739,8 +5739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5765,7 +5765,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>50</v>
@@ -5831,46 +5831,46 @@
         <v>111</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>172</v>
       </c>
       <c r="G4" s="25"/>
       <c r="H4" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M4" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q4" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="R4" s="28" t="s">
         <v>197</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>198</v>
       </c>
       <c r="S4" s="25"/>
       <c r="T4" s="25"/>
       <c r="U4" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="V4" s="28" t="s">
         <v>211</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>212</v>
       </c>
       <c r="X4" s="22"/>
       <c r="Y4" s="26" t="s">
@@ -5879,24 +5879,24 @@
     </row>
     <row r="5" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
@@ -5905,25 +5905,25 @@
         <v>121</v>
       </c>
       <c r="N5" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O5" s="25"/>
       <c r="P5" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q5" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="Q5" s="28" t="s">
+      <c r="R5" s="28" t="s">
         <v>235</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>236</v>
       </c>
       <c r="S5" s="25"/>
       <c r="T5" s="25"/>
       <c r="U5" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="V5" s="28" t="s">
         <v>238</v>
-      </c>
-      <c r="V5" s="28" t="s">
-        <v>239</v>
       </c>
       <c r="X5" s="25"/>
       <c r="Y5" s="27" t="s">
@@ -5938,7 +5938,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="25"/>
@@ -5968,7 +5968,7 @@
       <c r="V6" s="25"/>
       <c r="X6" s="29"/>
       <c r="Y6" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5976,10 +5976,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22"/>
@@ -6083,7 +6083,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -6199,7 +6199,7 @@
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
       <c r="L13" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M13" s="23" t="s">
         <v>121</v>
@@ -6254,17 +6254,17 @@
         <v>7</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="25"/>
       <c r="F15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>168</v>
       </c>
       <c r="H15" s="23" t="s">
         <v>116</v>
@@ -6275,23 +6275,23 @@
       <c r="J15" s="25"/>
       <c r="K15" s="25"/>
       <c r="L15" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M15" s="23" t="s">
         <v>121</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="23" t="s">
-        <v>136</v>
+        <v>242</v>
       </c>
       <c r="Q15" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="R15" s="28" t="s">
         <v>202</v>
-      </c>
-      <c r="R15" s="28" t="s">
-        <v>203</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -6322,7 +6322,7 @@
       <c r="N16" s="25"/>
       <c r="O16" s="22"/>
       <c r="P16" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q16" s="28"/>
       <c r="R16" s="28"/>
@@ -6336,19 +6336,19 @@
         <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" s="23" t="s">
         <v>115</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>116</v>
@@ -6368,16 +6368,16 @@
         <v>124</v>
       </c>
       <c r="O17" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R17" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S17" s="25"/>
       <c r="T17" s="25"/>
@@ -6416,21 +6416,21 @@
       </c>
       <c r="O18" s="25"/>
       <c r="P18" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R18" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S18" s="25"/>
       <c r="T18" s="25"/>
       <c r="U18" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="V18" s="28" t="s">
         <v>215</v>
-      </c>
-      <c r="V18" s="28" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="19" spans="2:25" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -6457,13 +6457,13 @@
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q19" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R19" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S19" s="25"/>
       <c r="T19" s="25"/>
@@ -6494,7 +6494,7 @@
       <c r="N20" s="25"/>
       <c r="O20" s="25"/>
       <c r="P20" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q20" s="28"/>
       <c r="R20" s="28"/>
@@ -6527,10 +6527,10 @@
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
       <c r="P21" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q21" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="R21" s="28"/>
       <c r="S21" s="25"/>
@@ -6565,18 +6565,18 @@
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
       <c r="P22" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q22" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="R22" s="28"/>
       <c r="S22" s="25"/>
       <c r="T22" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U22" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V22" s="25"/>
       <c r="W22" s="30"/>
@@ -6607,13 +6607,13 @@
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
       <c r="P23" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q23" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="R23" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>

</xml_diff>